<commit_message>
add v024 and v025
</commit_message>
<xml_diff>
--- a/TABLE/tabel-nominal.xlsx
+++ b/TABLE/tabel-nominal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\Probleme BAC 2009\TABLE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\Probleme-BAC-2009\TABLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999A9ACF-27CF-42F6-9788-B443A38C9EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5821F0-B595-4D2C-99F7-AEDBDE4BDF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -445,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,7 +680,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" s="7"/>
     </row>
@@ -689,7 +689,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26" s="7"/>
     </row>

</xml_diff>

<commit_message>
Revert "add v024 and v025"
This reverts commit 220cd96f7a02b80c1e533dd29574a2c70279f863.
</commit_message>
<xml_diff>
--- a/TABLE/tabel-nominal.xlsx
+++ b/TABLE/tabel-nominal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\Probleme-BAC-2009\TABLE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\Probleme BAC 2009\TABLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5821F0-B595-4D2C-99F7-AEDBDE4BDF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999A9ACF-27CF-42F6-9788-B443A38C9EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -445,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,7 +680,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25" s="7"/>
     </row>
@@ -689,7 +689,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26" s="7"/>
     </row>

</xml_diff>